<commit_message>
benin-tas: update all form
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Benin/bj_lf_pretas_3_resultat_fts_202009.xlsx
+++ b/LF/PreTAS/Benin/bj_lf_pretas_3_resultat_fts_202009.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\PreTAS\Benin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB44955-7F99-4EFD-8EF1-F2007FAB196E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22700E97-5545-42E2-8EFD-13971F0BA0E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -1107,10 +1107,10 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
+      <selection pane="bottomRight" activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>